<commit_message>
Add charts with log scale and save to pictures
</commit_message>
<xml_diff>
--- a/src/main/resources/outputs_comp/f2_out_out.xlsx
+++ b/src/main/resources/outputs_comp/f2_out_out.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuvus\Projects\tinyGPDataGenerator\src\main\resources\outputs_comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83BDBD6-9793-4668-B06B-A1FF6B051796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D27D6EE-FDD4-4430-B2E8-7B2AE6F6BEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1836,6 +1836,954 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>f(x) = sin(x) + cos(x)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Avg fit</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$A$1:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1779.117820052656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>332.03337417251407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171.3625865508032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>146.13480675587579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>279.40057203666862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138.37921961958671</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>172.92485106310761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>146.80560750317201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>148.15339177047099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>137.07375321320569</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>129.2310697052597</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>123.6296851116341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145.11183888340801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>584.16580571183169</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126.8110341765979</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>151.00511603164469</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>231.08401566328629</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>172.3130905202747</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2009.0513980345411</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>237.67625831160689</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>558.84806418182359</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>597.28455681531761</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>253.1217785787149</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>192.30147187666191</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355.94355132213951</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>503.78571906076269</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270.0831559532773</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>186.3364961977226</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>343.33831517581348</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220.99887880320389</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12769.004297739521</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1152.143352865186</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>377.07018201735872</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>99.054667473836986</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>173.61752595213829</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>91.885426900076936</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.222399990466783</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>104.3672872258383</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>172.0002191263238</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>137.91747074238279</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>148.5790504713157</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>121.6313367984869</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>114.2023095339549</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>110.63750104288179</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>127.13478903778019</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>117.7331738677927</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>111.53605076384621</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>79.263477513654749</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>217.00946718099581</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>131.81683052888661</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>193.79340862826831</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>83.541641673115933</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>357.0554780796457</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>72.230507342324373</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>152.98265334393571</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>181.88561687835809</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>209.66971222159751</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>385.73270976771391</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>79.31709454403952</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>86.843021747935737</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>121.6382917749135</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>88.272340044085567</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>153.64870484672301</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>88.548356743550173</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>104.00422704206891</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>112.7056309212023</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>10740.830741158319</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>94.754941972288975</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>180.16481114928129</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>162.27253277298931</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1110.9100165014449</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>124.5165001555782</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>205.52793950117751</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>725.62881027112212</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>384.59928942935733</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>107.0896808335881</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>883.01556278935163</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>126.4115951766493</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>134.8772110979078</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>620.0036918047673</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>318.20338436673001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>193.3623500144536</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>548.61403835948613</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1115.3162200537929</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>12347.998624753031</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>113.2454184754949</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>924.83772189367141</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1437.23150272313</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1400.3910982139039</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>629.19467550503464</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>760.89269373166201</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>167.57073891640661</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>618295.68869764335</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>289.36602102427588</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>563.17167011949641</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>271.26440123474362</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>372.72852868525479</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>349.90015447408132</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10784.98697333824</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>350.83037720346778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-985A-4FA4-A36F-3FDB93D10B47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Best fit</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$B$1:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>63.165098862354753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.017886623694757</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.111863279086343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.381478858237443</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.381478858237443</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.381478858237443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.470107907238898</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.838611326405783</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.141434740429062</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.656167038554209</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.72571769819217</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.72571769819217</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.72571769819217</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17.197138294502029</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.237481123708539</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.18814700847811</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.16552438821939</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.22294064577177</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.407924313118559</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.407924313118559</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.407924313118559</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.3041534718589292</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.9479605639211366</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.9479605639211366</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.34357647797711</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1397556931488486</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.8714651991735476</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.5671479188616448</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.4958405489498396</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.1356512594386841</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.9791951018783429</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.8126416220335142</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.684059714776668</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.3892466890766721</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.3864163022743838</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.309761544013206</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.308372439287365</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.2802162794556602</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.202706908565943</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.9995744024000319</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.9995744024000319</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.9988478562744931</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.9901910445329158</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.9879670401599889</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.9286308703759212</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.9273452604200401</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.914093396913612</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.8562429973740611</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.8562429973740611</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.844322722052381</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.7897701546315972</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.7560623765950911</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.7202748560111978</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.6820288943583419</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.6051676895068909</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.6051676895068909</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.6051676895068909</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.6051676895068909</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.6051676895068909</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.6013305405818201</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.5575389583514689</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.5002795086311611</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.4355421852521308</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.380438696763834</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.380438696763834</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.3804278562418291</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.3492477695733629</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.3404722124887249</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.3404722124887249</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.339246262827384</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.312451245677432</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.312451245677432</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.3124369835900822</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.3011308352433271</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.2827200111103392</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.282509360286225</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.2805941286911859</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.2506157862068021</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.217162810944143</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.2118115541606191</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.2011034332318808</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.1799235427754931</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.1799235427754931</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.1796710048647081</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.166867936234397</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.161173069820574</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.1357417137562789</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.1295919877163678</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.062771094582569</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.050086269155214</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.050086269155214</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.0276797255286212</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.0105793392106479</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.943549118978622</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.934797360852454</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-985A-4FA4-A36F-3FDB93D10B47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="812738496"/>
+        <c:axId val="814796896"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="812738496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814796896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="814796896"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812738496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1916,6 +2864,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2433,6 +3421,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3019,6 +4523,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A8A8CD-7609-4EBF-A41E-0C36118EC006}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3314,8 +4856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>